<commit_message>
added new bigquery tcs
</commit_message>
<xml_diff>
--- a/datf_core/test/testprotocol/testprotocol.xlsx
+++ b/datf_core/test/testprotocol/testprotocol.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspaces\GitHub\QE_ATF\test\testprotocol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspaces\GitHub\QE_ATF\datf_core\test\testprotocol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7281F80-D5DE-4119-B5CB-11B7BEAA2144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190BE9D8-4161-4A2B-B34F-D9DC26F0C667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -129,9 +129,6 @@
     <t>/app/test/results/</t>
   </si>
   <si>
-    <t>testcase22_bigquery_mysql_match</t>
-  </si>
-  <si>
     <t>testcase19_oracle_mysql_match_manual</t>
   </si>
   <si>
@@ -156,9 +153,6 @@
     <t>testcase27_csv_csv_bigdata_match</t>
   </si>
   <si>
-    <t>testcase21_mysql_csv_match</t>
-  </si>
-  <si>
     <t>testcase26_names_fullname_etljob</t>
   </si>
   <si>
@@ -178,6 +172,12 @@
   </si>
   <si>
     <t>multiple</t>
+  </si>
+  <si>
+    <t>testcase22_bigquery_bigquery_match</t>
+  </si>
+  <si>
+    <t>testcase21_csv_bigquery_match</t>
   </si>
 </sst>
 </file>
@@ -580,7 +580,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -588,7 +588,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -632,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333783BD-EC86-4502-A630-819DEFF8253B}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,7 +655,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -670,7 +670,7 @@
         <v>/app/test/testcases/testcase1_parquet_parquet_mismatch.xlsx</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -685,7 +685,7 @@
         <v>/app/test/testcases/testcase2_parquet_parquet_match.xlsx</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -700,7 +700,7 @@
         <v>/app/test/testcases/testcase3_csv_csv_match.xlsx</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -715,7 +715,7 @@
         <v>/app/test/testcases/testcase4_csv_csv_mismatch.xlsx</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -730,7 +730,7 @@
         <v>/app/test/testcases/testcase5_csv_parquet_match.xlsx</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -745,7 +745,7 @@
         <v>/app/test/testcases/testcase6_csv_parquet_mismatch.xlsx</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -760,7 +760,7 @@
         <v>/app/test/testcases/testcase7_json_json_mismatch.xlsx</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -775,7 +775,7 @@
         <v>/app/test/testcases/testcase8_json_json_match.xlsx</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -790,7 +790,7 @@
         <v>/app/test/testcases/testcase9_json_parquet_match.xlsx</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -805,7 +805,7 @@
         <v>/app/test/testcases/testcase10_json_parquet_mismatch.xlsx</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -820,7 +820,7 @@
         <v>/app/test/testcases/testcase11_parquet_parquet_match_manual.xlsx</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -835,7 +835,7 @@
         <v>/app/test/testcases/testcase12_parquet_parquet_mismatch_manual.xlsx</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -850,7 +850,7 @@
         <v>/app/test/testcases/testcase13_csv_parquet_match_manuel.xlsx</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -865,7 +865,7 @@
         <v>/app/test/testcases/testcase14_csv_parquet_mismatch_manual.xlsx</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -880,7 +880,7 @@
         <v>/app/test/testcases/testcase15_parquet_parquet_match_likeobject.xlsx</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -895,7 +895,7 @@
         <v>/app/test/testcases/testcase16_parquet_parquet_mismatch_likeobject.xlsx</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -910,7 +910,7 @@
         <v>/app/test/testcases/testcase17_dbtable_dbtable_match_likeobject.xlsx</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -925,7 +925,7 @@
         <v>/app/test/testcases/testcase18_parquet_dbtable_match_likeobject.xlsx</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -933,14 +933,14 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="4" t="str">
         <f t="shared" si="0"/>
         <v>/app/test/testcases/testcase19_oracle_mysql_match_manual.xlsx</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -948,14 +948,14 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="4" t="str">
         <f t="shared" si="0"/>
         <v>/app/test/testcases/testcase20_oracle_bigquery_match_manual.xlsx</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -963,14 +963,14 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C22" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>/app/test/testcases/testcase21_mysql_csv_match.xlsx</v>
+        <v>/app/test/testcases/testcase21_csv_bigquery_match.xlsx</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -978,14 +978,14 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C23" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>/app/test/testcases/testcase22_bigquery_mysql_match.xlsx</v>
+        <v>/app/test/testcases/testcase22_bigquery_bigquery_match.xlsx</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -993,14 +993,14 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" s="4" t="str">
         <f t="shared" si="0"/>
         <v>/app/test/testcases/testcase23_parquet_snowflake_mismatch.xlsx</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1008,14 +1008,14 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C25" s="4" t="str">
         <f t="shared" si="0"/>
         <v>/app/test/testcases/testcase24_snowflake_snowflake_etljob.xlsx</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1023,14 +1023,14 @@
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" s="4" t="str">
         <f t="shared" si="0"/>
         <v>/app/test/testcases/testcase25_oracle_oracle_etljob.xlsx</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1038,14 +1038,14 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C27" s="4" t="str">
         <f>_xlfn.CONCAT("/app/test/testcases/",B27,".xlsx")</f>
         <v>/app/test/testcases/testcase26_names_fullname_etljob.xlsx</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1053,14 +1053,14 @@
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28" s="4" t="str">
         <f>_xlfn.CONCAT("/app/test/testcases/",B28,".xlsx")</f>
         <v>/app/test/testcases/testcase27_csv_csv_bigdata_match.xlsx</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1068,14 +1068,14 @@
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C29" s="4" t="str">
         <f>_xlfn.CONCAT("/app/test/testcases/",B29,".xlsx")</f>
         <v>/app/test/testcases/testcase28_manual_sql_notifications.xlsx</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1083,14 +1083,14 @@
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C30" s="4" t="str">
         <f>_xlfn.CONCAT("/app/test/testcases/",B30,".xlsx")</f>
         <v>/app/test/testcases/testcase29_manual_sql_fullname.xlsx</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1098,14 +1098,14 @@
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C31" s="4" t="str">
         <f>_xlfn.CONCAT("/app/test/testcases/",B31,".xlsx")</f>
         <v>/app/test/testcases/testcase30_csv_csv_3mill50cols_content.xlsx</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated Notebook and rootpaths
</commit_message>
<xml_diff>
--- a/datf_core/test/testprotocol/testprotocol.xlsx
+++ b/datf_core/test/testprotocol/testprotocol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspaces\GitHub\DATF_Other\Databricks\QE_ATF\datf_core\test\testprotocol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\McKessoon\Azure Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D529C3-EF70-44E1-A0E9-31B5953CC14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE09148-4927-41CF-9A6F-ED3728AEA86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="protocol" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="50">
   <si>
     <t>Sno.</t>
   </si>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t>testcase31_delta_parquet_manual</t>
+  </si>
+  <si>
+    <t>testcase32_adls_parquet_to_delta_auto</t>
+  </si>
+  <si>
+    <t>testcase33_adls_parquet_adls_csv_auto</t>
   </si>
 </sst>
 </file>
@@ -636,10 +642,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333783BD-EC86-4502-A630-819DEFF8253B}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,7 +1053,7 @@
         <v>42</v>
       </c>
       <c r="C27" s="4" t="str">
-        <f t="shared" ref="C27:C32" si="2">_xlfn.CONCAT("test/testcases/",B27,".xlsx")</f>
+        <f t="shared" ref="C27:C34" si="2">_xlfn.CONCAT("test/testcases/",B27,".xlsx")</f>
         <v>test/testcases/testcase26_names_fullname_etljob.xlsx</v>
       </c>
       <c r="D27" s="6" t="s">
@@ -1127,6 +1133,36 @@
       </c>
       <c r="D32" s="6" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>32</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>test/testcases/testcase32_adls_parquet_to_delta_auto.xlsx</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>33</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>test/testcases/testcase33_adls_parquet_adls_csv_auto.xlsx</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>